<commit_message>
add SendBird chatbox AI
</commit_message>
<xml_diff>
--- a/ProjectManagement.xlsx
+++ b/ProjectManagement.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dự Án Tốt Nghiệp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraduationProject\NanaWebFood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D985F4-A57D-4ABB-B001-1275AA0117B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA009E86-1BD7-4B7D-BB11-EDBD15E82E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="82">
   <si>
     <t xml:space="preserve"> Project : Web bán thức ăn nhanh trực tuyến</t>
   </si>
@@ -279,6 +279,27 @@
   </si>
   <si>
     <t>Chức năng trung bình mà mỗi người cần thực hiện</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Undone</t>
+  </si>
+  <si>
+    <t>Doing</t>
+  </si>
+  <si>
+    <t>Excluded</t>
+  </si>
+  <si>
+    <t>Chức năng đã hoàn thành</t>
+  </si>
+  <si>
+    <t>Chức năng chưa hoàn thành</t>
+  </si>
+  <si>
+    <t>Chức năng bị loại bỏ</t>
   </si>
 </sst>
 </file>
@@ -387,7 +408,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -423,11 +444,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -471,21 +503,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -506,6 +523,24 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -785,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="D22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -797,51 +832,51 @@
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" customWidth="1"/>
     <col min="7" max="7" width="17.42578125" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="43.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="43.15" customHeight="1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19" t="s">
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="17"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="1:10" ht="25.15" customHeight="1">
-      <c r="A3" s="20"/>
+      <c r="A3" s="28"/>
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
@@ -851,12 +886,12 @@
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="17"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:10" ht="120">
       <c r="A4" s="3">
@@ -879,7 +914,9 @@
       <c r="H4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="3"/>
+      <c r="I4" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="38.25">
       <c r="A5" s="3">
@@ -903,7 +940,9 @@
       <c r="H5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="38.25">
       <c r="A6" s="3">
@@ -927,7 +966,9 @@
       <c r="H6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="25.5">
       <c r="A7" s="3">
@@ -951,7 +992,9 @@
       <c r="H7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="3"/>
+      <c r="I7" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="38.25">
       <c r="A8" s="3">
@@ -975,7 +1018,9 @@
       <c r="H8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="3"/>
+      <c r="I8" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="38.25">
       <c r="A9" s="3">
@@ -999,7 +1044,9 @@
       <c r="H9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="3"/>
+      <c r="I9" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="38.25">
       <c r="A10" s="3">
@@ -1023,7 +1070,9 @@
       <c r="H10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="3"/>
+      <c r="I10" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="51">
       <c r="A11" s="3">
@@ -1047,7 +1096,9 @@
       <c r="H11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="3"/>
+      <c r="I11" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="38.25">
       <c r="A12" s="3">
@@ -1071,7 +1122,9 @@
       <c r="H12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="7"/>
+      <c r="I12" s="7" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="38.25">
       <c r="A13" s="3">
@@ -1095,7 +1148,9 @@
       <c r="H13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="7"/>
+      <c r="I13" s="7" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="14" spans="1:10" ht="38.25">
       <c r="A14" s="3">
@@ -1119,7 +1174,9 @@
       <c r="H14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="9"/>
+      <c r="I14" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="38.25">
       <c r="A15" s="3">
@@ -1143,7 +1200,9 @@
       <c r="H15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="9"/>
+      <c r="I15" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="16" spans="1:10" ht="30">
       <c r="A16" s="3">
@@ -1153,7 +1212,7 @@
       <c r="B16" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="18" t="s">
         <v>71</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -1167,7 +1226,9 @@
       <c r="H16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="9"/>
+      <c r="I16" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="38.25">
       <c r="A17" s="3">
@@ -1191,7 +1252,9 @@
       <c r="H17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="9"/>
+      <c r="I17" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="51">
       <c r="A18" s="3">
@@ -1215,7 +1278,9 @@
       <c r="H18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I18" s="9"/>
+      <c r="I18" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="75">
       <c r="A19" s="3">
@@ -1225,7 +1290,7 @@
       <c r="B19" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="23" t="s">
         <v>72</v>
       </c>
       <c r="D19" s="14" t="s">
@@ -1239,7 +1304,9 @@
       <c r="H19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I19" s="9"/>
+      <c r="I19" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="72.75" customHeight="1">
       <c r="A20" s="3">
@@ -1263,7 +1330,9 @@
       <c r="H20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I20" s="9"/>
+      <c r="I20" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="63.75" customHeight="1">
       <c r="A21" s="3">
@@ -1273,7 +1342,7 @@
       <c r="B21" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="24" t="s">
         <v>73</v>
       </c>
       <c r="D21" s="5" t="s">
@@ -1287,7 +1356,9 @@
       <c r="H21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="9"/>
+      <c r="I21" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="22" spans="1:9" ht="48.75" customHeight="1">
       <c r="A22" s="3">
@@ -1311,7 +1382,9 @@
       <c r="H22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I22" s="9"/>
+      <c r="I22" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="23" spans="1:9" ht="42" customHeight="1">
       <c r="A23" s="3">
@@ -1335,7 +1408,7 @@
       <c r="H23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I23" s="9"/>
+      <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9" ht="51">
       <c r="A24" s="3">
@@ -1359,7 +1432,9 @@
       <c r="H24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I24" s="9"/>
+      <c r="I24" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="38.25">
       <c r="A25" s="3">
@@ -1383,7 +1458,9 @@
       <c r="H25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I25" s="9"/>
+      <c r="I25" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="25.5">
       <c r="A26" s="3">
@@ -1407,23 +1484,25 @@
       <c r="H26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I26" s="9"/>
+      <c r="I26" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="27" spans="1:9" ht="45">
       <c r="A27" s="3">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="25" t="s">
+      <c r="D27" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="22" t="s">
         <v>61</v>
       </c>
       <c r="F27" s="9"/>
@@ -1431,37 +1510,60 @@
       <c r="H27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I27" s="9"/>
+      <c r="I27" s="3" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="17" t="s">
         <v>62</v>
       </c>
       <c r="C28">
-        <f>COUNTIF(E4:E26, "=3")</f>
+        <f>COUNTIF(E4:E27,"=3")</f>
         <v>10</v>
       </c>
+      <c r="H28" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="I28">
+        <f>COUNTIF(I4:I27,"DONE")</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="29" spans="1:9">
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="17" t="s">
         <v>63</v>
       </c>
       <c r="C29">
         <f>COUNTIF(E4:E27,"=2")</f>
         <v>6</v>
       </c>
+      <c r="H29" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="I29">
+        <f>COUNTIF(I4:I27,"Undone")</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="17" t="s">
         <v>64</v>
       </c>
       <c r="C30">
         <f>COUNTIF(E4:E27,"=1")</f>
         <v>7</v>
       </c>
+      <c r="H30" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="I30">
+        <f>COUNTIF(I4:I27,"Excluded")</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:9">
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="17" t="s">
         <v>65</v>
       </c>
       <c r="C31">
@@ -1470,7 +1572,7 @@
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="17" t="s">
         <v>66</v>
       </c>
       <c r="C32">
@@ -1479,7 +1581,7 @@
       </c>
     </row>
     <row r="33" spans="2:3" ht="30">
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="21" t="s">
         <v>67</v>
       </c>
       <c r="C33">
@@ -1488,7 +1590,7 @@
       </c>
     </row>
     <row r="34" spans="2:3" ht="30">
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="21" t="s">
         <v>68</v>
       </c>
       <c r="C34">
@@ -1497,7 +1599,7 @@
       </c>
     </row>
     <row r="35" spans="2:3" ht="30">
-      <c r="B35" s="26" t="s">
+      <c r="B35" s="21" t="s">
         <v>74</v>
       </c>
       <c r="C35">
@@ -1506,7 +1608,7 @@
       </c>
     </row>
     <row r="36" spans="2:3" ht="30">
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="21" t="s">
         <v>69</v>
       </c>
       <c r="C36">
@@ -1515,7 +1617,7 @@
       </c>
     </row>
     <row r="37" spans="2:3" ht="45">
-      <c r="B37" s="26" t="s">
+      <c r="B37" s="21" t="s">
         <v>70</v>
       </c>
       <c r="C37">
@@ -1536,6 +1638,42 @@
     <mergeCell ref="I2:I3"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:E26">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25:E26">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E23">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -1547,44 +1685,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
+  <conditionalFormatting sqref="E13">
     <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25:E26">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E23">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
-    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1594,7 +1696,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1606,7 +1708,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1614,6 +1716,30 @@
         <color rgb="FFFF7128"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:I27">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="between">
+      <formula>"Done"</formula>
+      <formula>"Undone"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="formula" val="&quot;Done&quot;"/>
+        <cfvo type="formula" val="&quot;Excluded&quot;"/>
+        <cfvo type="formula" val="&quot;Undone&quot;"/>
+        <color theme="9" tint="0.39997558519241921"/>
+        <color rgb="FFFF0000"/>
+        <color theme="7" tint="0.39997558519241921"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>